<commit_message>
Ajout PIN 6 pompe à vide dans pin_mapping.h et PinMapping.xlsx
</commit_message>
<xml_diff>
--- a/PinMapping.xlsx
+++ b/PinMapping.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t xml:space="preserve">Pin</t>
   </si>
@@ -52,10 +52,16 @@
     <t xml:space="preserve">PWM_G</t>
   </si>
   <si>
+    <t xml:space="preserve">POMPE</t>
+  </si>
+  <si>
     <t xml:space="preserve">DIR_D</t>
   </si>
   <si>
     <t xml:space="preserve">PWM_D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POMPE_A_VIDE</t>
   </si>
   <si>
     <t xml:space="preserve">SS</t>
@@ -122,7 +128,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -161,6 +167,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCFF"/>
+        <bgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA9D18E"/>
         <bgColor rgb="FFC5E0B4"/>
       </patternFill>
@@ -172,7 +184,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -188,9 +200,9 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="medium"/>
-      <top style="medium"/>
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
       <bottom/>
       <diagonal/>
     </border>
@@ -209,31 +221,38 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="medium"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
       <left style="medium"/>
       <right style="medium"/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="medium"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="medium"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="medium"/>
-      <top/>
-      <bottom style="medium"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -276,7 +295,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -317,11 +336,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -329,15 +352,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -353,7 +380,7 @@
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFFCCFF"/>
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
@@ -421,19 +448,19 @@
   <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.55"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.3886639676113"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.5303643724696"/>
     <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.7813765182186"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -444,7 +471,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="n">
         <v>0</v>
       </c>
@@ -455,7 +482,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="n">
         <v>1</v>
       </c>
@@ -466,7 +493,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="n">
         <v>2</v>
       </c>
@@ -477,12 +504,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="n">
         <v>3</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>9</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -490,7 +520,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -498,14 +528,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="7"/>
+      <c r="B8" s="12" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="n">
@@ -525,50 +557,50 @@
       </c>
       <c r="B11" s="7"/>
     </row>
-    <row r="12" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="n">
         <v>10</v>
       </c>
-      <c r="B12" s="11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="n">
         <v>11</v>
       </c>
-      <c r="B13" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="n">
         <v>12</v>
       </c>
-      <c r="B14" s="11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="n">
         <v>13</v>
       </c>
-      <c r="B15" s="11"/>
-    </row>
-    <row r="16" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="13"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="n">
         <v>14</v>
       </c>
-      <c r="B16" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="n">
         <v>15</v>
       </c>
-      <c r="B17" s="11" t="s">
-        <v>16</v>
+      <c r="B17" s="13" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -599,32 +631,32 @@
       <c r="A22" s="6" t="n">
         <v>20</v>
       </c>
-      <c r="B22" s="12" t="s">
-        <v>17</v>
+      <c r="B22" s="14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="n">
         <v>21</v>
       </c>
-      <c r="B23" s="12" t="s">
-        <v>18</v>
+      <c r="B23" s="14" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="n">
         <v>22</v>
       </c>
-      <c r="B24" s="12" t="s">
-        <v>19</v>
+      <c r="B24" s="14" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="n">
         <v>23</v>
       </c>
-      <c r="B25" s="12" t="s">
-        <v>20</v>
+      <c r="B25" s="14" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -685,13 +717,13 @@
       <c r="A35" s="6" t="n">
         <v>33</v>
       </c>
-      <c r="B35" s="13"/>
+      <c r="B35" s="15"/>
     </row>
     <row r="36" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="6" t="n">
         <v>34</v>
       </c>
-      <c r="B36" s="13"/>
+      <c r="B36" s="15"/>
     </row>
     <row r="37" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="6" t="n">
@@ -718,10 +750,10 @@
       <c r="B40" s="7"/>
     </row>
     <row r="41" customFormat="false" ht="15.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="14" t="n">
+      <c r="A41" s="16" t="n">
         <v>39</v>
       </c>
-      <c r="B41" s="15"/>
+      <c r="B41" s="17"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Mise à 25% du PWN de la pompe à vide
</commit_message>
<xml_diff>
--- a/PinMapping.xlsx
+++ b/PinMapping.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t xml:space="preserve">Pin</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t xml:space="preserve">POMPE_A_VIDE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PWM_POMPE</t>
   </si>
   <si>
     <t xml:space="preserve">SS</t>
@@ -295,7 +298,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -345,6 +348,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -448,15 +455,15 @@
   <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.55"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.7449392712551"/>
     <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.7813765182186"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.8866396761134"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -539,11 +546,13 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="n">
         <v>7</v>
       </c>
-      <c r="B9" s="7"/>
+      <c r="B9" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="n">
@@ -561,46 +570,46 @@
       <c r="A12" s="6" t="n">
         <v>10</v>
       </c>
-      <c r="B12" s="13" t="s">
-        <v>14</v>
+      <c r="B12" s="14" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="n">
         <v>11</v>
       </c>
-      <c r="B13" s="13" t="s">
-        <v>15</v>
+      <c r="B13" s="14" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="n">
         <v>12</v>
       </c>
-      <c r="B14" s="13" t="s">
-        <v>16</v>
+      <c r="B14" s="14" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="n">
         <v>13</v>
       </c>
-      <c r="B15" s="13"/>
+      <c r="B15" s="14"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="n">
         <v>14</v>
       </c>
-      <c r="B16" s="13" t="s">
-        <v>17</v>
+      <c r="B16" s="14" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="n">
         <v>15</v>
       </c>
-      <c r="B17" s="13" t="s">
-        <v>18</v>
+      <c r="B17" s="14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -631,32 +640,32 @@
       <c r="A22" s="6" t="n">
         <v>20</v>
       </c>
-      <c r="B22" s="14" t="s">
-        <v>19</v>
+      <c r="B22" s="15" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="n">
         <v>21</v>
       </c>
-      <c r="B23" s="14" t="s">
-        <v>20</v>
+      <c r="B23" s="15" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="n">
         <v>22</v>
       </c>
-      <c r="B24" s="14" t="s">
-        <v>21</v>
+      <c r="B24" s="15" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="n">
         <v>23</v>
       </c>
-      <c r="B25" s="14" t="s">
-        <v>22</v>
+      <c r="B25" s="15" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -717,13 +726,13 @@
       <c r="A35" s="6" t="n">
         <v>33</v>
       </c>
-      <c r="B35" s="15"/>
+      <c r="B35" s="16"/>
     </row>
     <row r="36" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="6" t="n">
         <v>34</v>
       </c>
-      <c r="B36" s="15"/>
+      <c r="B36" s="16"/>
     </row>
     <row r="37" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="6" t="n">
@@ -750,10 +759,10 @@
       <c r="B40" s="7"/>
     </row>
     <row r="41" customFormat="false" ht="15.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="16" t="n">
+      <c r="A41" s="17" t="n">
         <v>39</v>
       </c>
-      <c r="B41" s="17"/>
+      <c r="B41" s="18"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Mise à 25% du PWN de la pompe à vide + modification de PinMapping.xlsx
</commit_message>
<xml_diff>
--- a/PinMapping.xlsx
+++ b/PinMapping.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t xml:space="preserve">Pin</t>
   </si>
@@ -59,9 +59,6 @@
   </si>
   <si>
     <t xml:space="preserve">PWM_D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">POMPE_A_VIDE</t>
   </si>
   <si>
     <t xml:space="preserve">PWM_POMPE</t>
@@ -351,7 +348,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -461,9 +458,9 @@
   <sheetFormatPr defaultRowHeight="14.55"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.9595141700405"/>
     <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.8866396761134"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.995951417004"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -550,9 +547,7 @@
       <c r="A9" s="6" t="n">
         <v>7</v>
       </c>
-      <c r="B9" s="13" t="s">
-        <v>14</v>
-      </c>
+      <c r="B9" s="13"/>
     </row>
     <row r="10" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="n">
@@ -571,7 +566,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -579,7 +574,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -587,7 +582,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -601,7 +596,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -609,7 +604,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -641,7 +636,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -649,7 +644,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -657,7 +652,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -665,7 +660,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Pin pompe 6 --> 9
</commit_message>
<xml_diff>
--- a/PinMapping.xlsx
+++ b/PinMapping.xlsx
@@ -295,7 +295,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -345,10 +345,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -452,15 +448,15 @@
   <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.55"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.9595141700405"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.1740890688259"/>
     <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.1012145748988"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -539,15 +535,12 @@
       <c r="A8" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="12" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="n">
         <v>7</v>
       </c>
-      <c r="B9" s="13"/>
+      <c r="B9" s="7"/>
     </row>
     <row r="10" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="n">
@@ -555,17 +548,19 @@
       </c>
       <c r="B10" s="7"/>
     </row>
-    <row r="11" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="n">
         <v>9</v>
       </c>
-      <c r="B11" s="7"/>
+      <c r="B11" s="12" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="n">
         <v>10</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="13" t="s">
         <v>14</v>
       </c>
     </row>
@@ -573,7 +568,7 @@
       <c r="A13" s="6" t="n">
         <v>11</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="13" t="s">
         <v>15</v>
       </c>
     </row>
@@ -581,7 +576,7 @@
       <c r="A14" s="6" t="n">
         <v>12</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="13" t="s">
         <v>16</v>
       </c>
     </row>
@@ -589,13 +584,13 @@
       <c r="A15" s="6" t="n">
         <v>13</v>
       </c>
-      <c r="B15" s="14"/>
+      <c r="B15" s="13"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="n">
         <v>14</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="13" t="s">
         <v>17</v>
       </c>
     </row>
@@ -603,7 +598,7 @@
       <c r="A17" s="6" t="n">
         <v>15</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="13" t="s">
         <v>18</v>
       </c>
     </row>
@@ -635,7 +630,7 @@
       <c r="A22" s="6" t="n">
         <v>20</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="14" t="s">
         <v>19</v>
       </c>
     </row>
@@ -643,7 +638,7 @@
       <c r="A23" s="6" t="n">
         <v>21</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="14" t="s">
         <v>20</v>
       </c>
     </row>
@@ -651,7 +646,7 @@
       <c r="A24" s="6" t="n">
         <v>22</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="14" t="s">
         <v>21</v>
       </c>
     </row>
@@ -659,7 +654,7 @@
       <c r="A25" s="6" t="n">
         <v>23</v>
       </c>
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="14" t="s">
         <v>22</v>
       </c>
     </row>
@@ -721,13 +716,13 @@
       <c r="A35" s="6" t="n">
         <v>33</v>
       </c>
-      <c r="B35" s="16"/>
+      <c r="B35" s="15"/>
     </row>
     <row r="36" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="6" t="n">
         <v>34</v>
       </c>
-      <c r="B36" s="16"/>
+      <c r="B36" s="15"/>
     </row>
     <row r="37" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="6" t="n">
@@ -754,10 +749,10 @@
       <c r="B40" s="7"/>
     </row>
     <row r="41" customFormat="false" ht="15.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="17" t="n">
+      <c r="A41" s="16" t="n">
         <v>39</v>
       </c>
-      <c r="B41" s="18"/>
+      <c r="B41" s="17"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
LED d'état Mise à jour du README Corrections mineures et un bullshit qui traînait
</commit_message>
<xml_diff>
--- a/PinMapping.xlsx
+++ b/PinMapping.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t xml:space="preserve">Pin</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t xml:space="preserve">A_LEFT_ENCODER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED D’ETAT</t>
   </si>
 </sst>
 </file>
@@ -447,17 +450,17 @@
   </sheetPr>
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.55"/>
+  <sheetFormatPr defaultRowHeight="14.55" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.1740890688259"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.1012145748988"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -698,7 +701,9 @@
       <c r="A32" s="6" t="n">
         <v>30</v>
       </c>
-      <c r="B32" s="7"/>
+      <c r="B32" s="7" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="6" t="n">
@@ -757,7 +762,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
pinmapping->SCK, readme, serveur initialisé au bon endroit pour faire plaisir à CLion
</commit_message>
<xml_diff>
--- a/PinMapping.xlsx
+++ b/PinMapping.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t xml:space="preserve">Pin</t>
   </si>
@@ -28,7 +28,7 @@
     <t xml:space="preserve">Usage</t>
   </si>
   <si>
-    <t xml:space="preserve">ETH</t>
+    <t xml:space="preserve">ETH(SPI0)</t>
   </si>
   <si>
     <t xml:space="preserve">RX1</t>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t xml:space="preserve">MISO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCK</t>
   </si>
   <si>
     <t xml:space="preserve">RST</t>
@@ -450,11 +453,11 @@
   </sheetPr>
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.55" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.55" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.17"/>
@@ -587,14 +590,16 @@
       <c r="A15" s="6" t="n">
         <v>13</v>
       </c>
-      <c r="B15" s="13"/>
+      <c r="B15" s="13" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="n">
         <v>14</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -602,7 +607,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -634,7 +639,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -642,7 +647,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -650,7 +655,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -658,7 +663,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -702,7 +707,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Ajout des ordres pour les électrovannes Définition des pins Mise à jour du pin_mapping
</commit_message>
<xml_diff>
--- a/PinMapping.xlsx
+++ b/PinMapping.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t xml:space="preserve">Pin</t>
   </si>
@@ -58,34 +58,43 @@
     <t xml:space="preserve">DIR_D</t>
   </si>
   <si>
+    <t xml:space="preserve">Elec-Vane</t>
+  </si>
+  <si>
     <t xml:space="preserve">PWM_D</t>
   </si>
   <si>
+    <t xml:space="preserve">B_RIGHT_ENCODER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A_RIGHT_ENCODER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOSI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MISO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PWD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ELECTROVANNE_AV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ELECTROVANNE_AR</t>
+  </si>
+  <si>
     <t xml:space="preserve">PWM_POMPE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOSI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MISO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PWD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B_RIGHT_ENCODER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A_RIGHT_ENCODER</t>
   </si>
   <si>
     <t xml:space="preserve">B_LEFT_ENCODER</t>
@@ -134,7 +143,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -179,14 +188,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA9D18E"/>
-        <bgColor rgb="FFC5E0B4"/>
+        <fgColor rgb="FF009999"/>
+        <bgColor rgb="FF008080"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor rgb="FFFFE699"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA9D18E"/>
+        <bgColor rgb="FFC5E0B4"/>
       </patternFill>
     </fill>
   </fills>
@@ -301,7 +316,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -346,19 +361,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -398,7 +421,7 @@
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF009999"/>
       <rgbColor rgb="FFC9C9C9"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
@@ -454,13 +477,13 @@
   <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
+      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.55" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.55" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="8.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.57"/>
@@ -521,12 +544,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="n">
         <v>4</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>11</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -534,21 +560,26 @@
         <v>5</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="n">
         <v>6</v>
       </c>
+      <c r="B8" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="n">
         <v>7</v>
       </c>
-      <c r="B9" s="7"/>
-    </row>
-    <row r="10" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="n">
         <v>8</v>
       </c>
@@ -558,75 +589,79 @@
       <c r="A11" s="6" t="n">
         <v>9</v>
       </c>
-      <c r="B11" s="12" t="s">
-        <v>13</v>
-      </c>
+      <c r="B11" s="7"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="n">
         <v>10</v>
       </c>
-      <c r="B12" s="13" t="s">
-        <v>14</v>
+      <c r="B12" s="14" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="n">
         <v>11</v>
       </c>
-      <c r="B13" s="13" t="s">
-        <v>15</v>
+      <c r="B13" s="14" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="n">
         <v>12</v>
       </c>
-      <c r="B14" s="13" t="s">
-        <v>16</v>
+      <c r="B14" s="14" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="n">
         <v>13</v>
       </c>
-      <c r="B15" s="13" t="s">
-        <v>17</v>
+      <c r="B15" s="14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="n">
         <v>14</v>
       </c>
-      <c r="B16" s="13" t="s">
-        <v>18</v>
+      <c r="B16" s="14" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="n">
         <v>15</v>
       </c>
-      <c r="B17" s="13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="n">
         <v>16</v>
       </c>
-      <c r="B18" s="7"/>
+      <c r="B18" s="15" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="n">
         <v>17</v>
       </c>
-      <c r="B19" s="7"/>
-    </row>
-    <row r="20" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="n">
         <v>18</v>
       </c>
-      <c r="B20" s="7"/>
+      <c r="B20" s="16" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="n">
@@ -638,32 +673,28 @@
       <c r="A22" s="6" t="n">
         <v>20</v>
       </c>
-      <c r="B22" s="14" t="s">
-        <v>20</v>
-      </c>
+      <c r="B22" s="7"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="n">
         <v>21</v>
       </c>
-      <c r="B23" s="14" t="s">
-        <v>21</v>
-      </c>
+      <c r="B23" s="7"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="n">
         <v>22</v>
       </c>
-      <c r="B24" s="14" t="s">
-        <v>22</v>
+      <c r="B24" s="13" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="n">
         <v>23</v>
       </c>
-      <c r="B25" s="14" t="s">
-        <v>23</v>
+      <c r="B25" s="13" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -707,7 +738,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -726,13 +757,13 @@
       <c r="A35" s="6" t="n">
         <v>33</v>
       </c>
-      <c r="B35" s="15"/>
+      <c r="B35" s="17"/>
     </row>
     <row r="36" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="6" t="n">
         <v>34</v>
       </c>
-      <c r="B36" s="15"/>
+      <c r="B36" s="17"/>
     </row>
     <row r="37" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="6" t="n">
@@ -759,10 +790,10 @@
       <c r="B40" s="7"/>
     </row>
     <row r="41" customFormat="false" ht="15.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="16" t="n">
+      <c r="A41" s="18" t="n">
         <v>39</v>
       </c>
-      <c r="B41" s="17"/>
+      <c r="B41" s="19"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Singe proofing des électrovannes/pompe Remodification des pins Peut-être une ou deux bananes dans le tas
</commit_message>
<xml_diff>
--- a/PinMapping.xlsx
+++ b/PinMapping.xlsx
@@ -64,37 +64,37 @@
     <t xml:space="preserve">PWM_D</t>
   </si>
   <si>
+    <t xml:space="preserve">ELECTROVANNE_AV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ELECTROVANNE_AR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PWM_POMPE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOSI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MISO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PWD</t>
+  </si>
+  <si>
     <t xml:space="preserve">B_RIGHT_ENCODER</t>
   </si>
   <si>
     <t xml:space="preserve">A_RIGHT_ENCODER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOSI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MISO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PWD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ELECTROVANNE_AV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ELECTROVANNE_AR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PWM_POMPE</t>
   </si>
   <si>
     <t xml:space="preserve">B_LEFT_ENCODER</t>
@@ -194,14 +194,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA9D18E"/>
+        <bgColor rgb="FFC5E0B4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor rgb="FFFFE699"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA9D18E"/>
-        <bgColor rgb="FFC5E0B4"/>
       </patternFill>
     </fill>
   </fills>
@@ -369,19 +369,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="9" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="10" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -476,8 +476,8 @@
   </sheetPr>
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.55" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -567,101 +567,96 @@
       <c r="A8" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="13" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="n">
         <v>7</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="n">
         <v>8</v>
       </c>
-      <c r="B10" s="7"/>
+      <c r="B10" s="13" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="n">
         <v>9</v>
       </c>
-      <c r="B11" s="7"/>
+      <c r="B11" s="14" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="n">
         <v>10</v>
       </c>
-      <c r="B12" s="14" t="s">
-        <v>16</v>
+      <c r="B12" s="15" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="n">
         <v>11</v>
       </c>
-      <c r="B13" s="14" t="s">
-        <v>17</v>
+      <c r="B13" s="15" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="n">
         <v>12</v>
       </c>
-      <c r="B14" s="14" t="s">
-        <v>18</v>
+      <c r="B14" s="15" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="n">
         <v>13</v>
       </c>
-      <c r="B15" s="14" t="s">
-        <v>19</v>
+      <c r="B15" s="15" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="n">
         <v>14</v>
       </c>
-      <c r="B16" s="14" t="s">
-        <v>20</v>
+      <c r="B16" s="15" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="n">
         <v>15</v>
       </c>
-      <c r="B17" s="14" t="s">
-        <v>21</v>
+      <c r="B17" s="15" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="n">
         <v>16</v>
       </c>
-      <c r="B18" s="15" t="s">
-        <v>22</v>
-      </c>
+      <c r="B18" s="7"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="n">
         <v>17</v>
       </c>
-      <c r="B19" s="15" t="s">
-        <v>23</v>
-      </c>
+      <c r="B19" s="7"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="n">
         <v>18</v>
       </c>
-      <c r="B20" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="B20" s="7"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="n">
@@ -673,19 +668,23 @@
       <c r="A22" s="6" t="n">
         <v>20</v>
       </c>
-      <c r="B22" s="7"/>
+      <c r="B22" s="16" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="n">
         <v>21</v>
       </c>
-      <c r="B23" s="7"/>
+      <c r="B23" s="16" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="n">
         <v>22</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="16" t="s">
         <v>25</v>
       </c>
     </row>
@@ -693,7 +692,7 @@
       <c r="A25" s="6" t="n">
         <v>23</v>
       </c>
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="16" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>